<commit_message>
ml modelling largely completed
</commit_message>
<xml_diff>
--- a/Supporting Details.xlsx
+++ b/Supporting Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartgow/GitHub/Telecom_Customer_Targeting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6863FD9-6C42-1546-9F1B-BCA89655FADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F99F8F-E7FB-5F49-8879-32EA94A62893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="4460" windowWidth="34200" windowHeight="19960" xr2:uid="{09AE4682-5911-EC4F-8C4B-DB9B4E1CC59A}"/>
+    <workbookView xWindow="520" yWindow="540" windowWidth="34200" windowHeight="19960" xr2:uid="{09AE4682-5911-EC4F-8C4B-DB9B4E1CC59A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="76">
   <si>
     <t>ID</t>
   </si>
@@ -140,18 +140,9 @@
     <t xml:space="preserve">40k never contacted, then max is 871 days! </t>
   </si>
   <si>
-    <t>?? Entirely drop 'previous campaign' data</t>
-  </si>
-  <si>
     <t>??  Combine into a date? Or just use month</t>
   </si>
   <si>
-    <t>?? Just use month for last contact day and month</t>
-  </si>
-  <si>
-    <t>Very evenly split. So double-check if of any training value</t>
-  </si>
-  <si>
     <t>5 were marked as 'n' rather than 'no'. Amend</t>
   </si>
   <si>
@@ -185,18 +176,6 @@
     <t>- Table of each model and cst function / evaluation used</t>
   </si>
   <si>
-    <t>- clean data before split or only clean training split</t>
-  </si>
-  <si>
-    <t>- normalise, encode fit to train then aplly to tran and test split</t>
-  </si>
-  <si>
-    <t>?? SMOTE (Syhthetic Minority Over-Sampling Technique) - see 2002 paper</t>
-  </si>
-  <si>
-    <t>- create processing pipeline that cen be rerun on different datasets/splits</t>
-  </si>
-  <si>
     <t>?? Use of pipelines</t>
   </si>
   <si>
@@ -209,42 +188,27 @@
     <t>101 towns. Occurences are unbalanced: 6 occur over 1200 times, 95 between 350 to 50 times</t>
   </si>
   <si>
-    <t>?? Use SMOTE to balance</t>
-  </si>
-  <si>
     <t>40,000 (80%) are 0 to 60 balance, rest very small. Large outliers: 5 over 750</t>
   </si>
   <si>
     <t>A very small proportion (2%) in arrears</t>
   </si>
   <si>
-    <t>?? Of any training value</t>
-  </si>
-  <si>
     <t>5 catgeories, all very similar values</t>
   </si>
   <si>
-    <t>?? Of any training value .. Add back later?</t>
-  </si>
-  <si>
     <t>Categorical - Nominal</t>
   </si>
   <si>
     <t>40k unknown and 2k other.</t>
   </si>
   <si>
-    <t>Only approx 10k new contract, 20%</t>
-  </si>
-  <si>
     <t>Rows</t>
   </si>
   <si>
     <t>Columns</t>
   </si>
   <si>
-    <t>?? Resolve the unknowns</t>
-  </si>
-  <si>
     <t>2095 unknown</t>
   </si>
   <si>
@@ -263,25 +227,43 @@
     <t>329 unknown but a small proportion overall. So leave</t>
   </si>
   <si>
-    <t>?? Of any training value .. Add back later? But rebalance</t>
-  </si>
-  <si>
-    <t>Removed outliers &gt; 30 …. or use SMOTE instead</t>
-  </si>
-  <si>
     <t>Approx 1250 had more than 10 contacts made (2.5%). And max was 63. 76 outliers removed &gt;= 30</t>
   </si>
   <si>
     <t>Outlier of 275 was dropped. 40k not contacted, majority under 10 (96%)</t>
   </si>
   <si>
-    <t>Removed 5 outliers …. Better to use SMOTE instead</t>
-  </si>
-  <si>
     <t>RobustScaler used due to outliers and skewed data</t>
   </si>
   <si>
     <t>?? Which pre and post data item to show</t>
+  </si>
+  <si>
+    <t>NB: Dropped after first modelling attempt</t>
+  </si>
+  <si>
+    <t>Dropped originaly but then added back and predictions improved</t>
+  </si>
+  <si>
+    <t>Very evenly split. But left in</t>
+  </si>
+  <si>
+    <t>Only approx 10k new contract, 20% - Imbalanced. SMOTE did not help but used some model parameters to balance</t>
+  </si>
+  <si>
+    <t>Removed outliers &gt; 750. 5 - But no impact on model so keft</t>
+  </si>
+  <si>
+    <t>Removed outliers &gt; 30. 76. But no impact on model so left</t>
+  </si>
+  <si>
+    <t>Appled outliers but mad little diffeence goven scaling and balancing in the models …. !! An insight</t>
+  </si>
+  <si>
+    <t>?? So not sure what data changed to show now!</t>
+  </si>
+  <si>
+    <t>?? SMOTE (Synhthetic Minority Over-Sampling Technique) - see 2002 paper</t>
   </si>
 </sst>
 </file>
@@ -328,7 +310,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +335,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -452,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -483,8 +471,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -499,17 +485,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D66C882-9645-1941-AF96-E05FA87E8238}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -862,7 +851,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -876,10 +865,10 @@
         <v>22</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>23</v>
@@ -902,7 +891,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="14"/>
       <c r="G5" s="5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -912,15 +901,15 @@
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>57</v>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -935,10 +924,11 @@
       </c>
       <c r="E7" s="2"/>
       <c r="G7" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="25"/>
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
@@ -953,6 +943,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="25"/>
       <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
@@ -965,10 +956,11 @@
       <c r="E9" s="2"/>
       <c r="F9" s="14"/>
       <c r="G9" s="5" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="25"/>
       <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
@@ -983,6 +975,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="25"/>
       <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
@@ -992,12 +985,10 @@
       <c r="D11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>68</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="14"/>
       <c r="G11" s="5" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1010,15 +1001,14 @@
       <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="14"/>
       <c r="G12" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="25"/>
       <c r="B13" s="15" t="s">
         <v>8</v>
       </c>
@@ -1028,33 +1018,33 @@
       <c r="D13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" s="14"/>
+      <c r="E13" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="29"/>
       <c r="G13" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="25"/>
       <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>60</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="14"/>
       <c r="G14" s="5" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="25"/>
       <c r="B15" s="15" t="s">
         <v>10</v>
       </c>
@@ -1067,10 +1057,11 @@
       <c r="E15" s="2"/>
       <c r="F15" s="14"/>
       <c r="G15" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="25"/>
       <c r="B16" s="15" t="s">
         <v>11</v>
       </c>
@@ -1083,10 +1074,10 @@
       <c r="E16" s="2"/>
       <c r="F16" s="14"/>
       <c r="G16" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
         <v>12</v>
       </c>
@@ -1099,28 +1090,26 @@
       <c r="E17" s="2"/>
       <c r="F17" s="14"/>
       <c r="G17" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>62</v>
-      </c>
+      <c r="E18" s="2"/>
       <c r="F18" s="14"/>
-      <c r="G18" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
@@ -1130,15 +1119,14 @@
       <c r="D19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>62</v>
-      </c>
+      <c r="E19" s="2"/>
       <c r="F19" s="14"/>
       <c r="G19" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="25"/>
       <c r="B20" s="15" t="s">
         <v>15</v>
       </c>
@@ -1148,100 +1136,92 @@
       <c r="D20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="18" t="s">
-        <v>76</v>
+      <c r="E20" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>62</v>
-      </c>
+      <c r="E21" s="2"/>
       <c r="G21" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>62</v>
-      </c>
+      <c r="E22" s="2"/>
       <c r="G22" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="25"/>
       <c r="B23" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>62</v>
+      <c r="D23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="26" t="s">
-        <v>57</v>
-      </c>
+      <c r="E24" s="28"/>
       <c r="F24" s="13"/>
       <c r="G24" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
@@ -1251,139 +1231,132 @@
       <c r="D29" s="17">
         <v>20</v>
       </c>
-      <c r="G29" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="17">
-        <v>50579</v>
+      <c r="C30" s="31">
+        <v>50660</v>
       </c>
       <c r="D30" s="17">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C31" s="30">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C31" s="24">
         <f>C29-C30</f>
-        <v>83</v>
-      </c>
-      <c r="D31" s="30">
+        <v>2</v>
+      </c>
+      <c r="D31" s="24">
         <f>D29-D30</f>
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="24" t="s">
-        <v>40</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D38" s="22"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="23" t="s">
-        <v>49</v>
-      </c>
+      <c r="B39" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="21"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>50</v>
-      </c>
+      <c r="B40" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="21"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="20"/>
-      <c r="D41" s="23" t="s">
-        <v>52</v>
-      </c>
+      <c r="B41" s="18"/>
+      <c r="D41" s="21"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="20"/>
-      <c r="D43" s="23"/>
+        <v>59</v>
+      </c>
+      <c r="B43" s="18"/>
+      <c r="D43" s="21"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" s="23"/>
+      <c r="B44" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" s="21"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D45" s="23"/>
+      <c r="B45" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="21"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B46" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="23"/>
+      <c r="B46" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="21"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="20"/>
-      <c r="D47" s="23"/>
+      <c r="B47" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" s="21"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="20"/>
-      <c r="D48" s="23"/>
+      <c r="B48" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="21"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="20"/>
-      <c r="D49" s="23"/>
+      <c r="B49" s="18"/>
+      <c r="D49" s="21"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D50" s="22"/>
+        <v>41</v>
+      </c>
+      <c r="D50" s="20"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D51" s="22"/>
+        <v>42</v>
+      </c>
+      <c r="D51" s="20"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="22"/>
+        <v>75</v>
+      </c>
+      <c r="D52" s="20"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D53" s="22"/>
+        <v>43</v>
+      </c>
+      <c r="D53" s="20"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D54" s="22"/>
+        <v>44</v>
+      </c>
+      <c r="D54" s="20"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D55" s="22"/>
+        <v>46</v>
+      </c>
+      <c r="D55" s="20"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D56" s="22"/>
+      <c r="D56" s="20"/>
     </row>
     <row r="57" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B57" s="25"/>
+      <c r="B57" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ML assignmnet near final
</commit_message>
<xml_diff>
--- a/Supporting Details.xlsx
+++ b/Supporting Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartgow/GitHub/Telecom_Customer_Targeting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BA4122-4952-1A47-BDBB-F85A14FFB1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09DAF7F-5F83-4D44-895F-AC598343ECF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13780" yWindow="4380" windowWidth="34200" windowHeight="19960" xr2:uid="{09AE4682-5911-EC4F-8C4B-DB9B4E1CC59A}"/>
+    <workbookView xWindow="740" yWindow="6240" windowWidth="34200" windowHeight="19960" xr2:uid="{09AE4682-5911-EC4F-8C4B-DB9B4E1CC59A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -150,36 +150,12 @@
     <t>2 were marked as 'cell' rather than 'cellular'. Amend</t>
   </si>
   <si>
-    <t>????</t>
-  </si>
-  <si>
-    <t>- Table of each model and hyperparameters chosed</t>
-  </si>
-  <si>
     <t>Feature Selection Approach Taken</t>
   </si>
   <si>
     <t>Insights'</t>
   </si>
   <si>
-    <t>References</t>
-  </si>
-  <si>
-    <t>?? CRISP</t>
-  </si>
-  <si>
-    <t>?? Scikit-learn docs</t>
-  </si>
-  <si>
-    <t>?? Data cleaning approaches</t>
-  </si>
-  <si>
-    <t>- Table of each model and cst function / evaluation used</t>
-  </si>
-  <si>
-    <t>?? Use of pipelines</t>
-  </si>
-  <si>
     <t>Variables - Acttions &amp; Questions</t>
   </si>
   <si>
@@ -216,12 +192,6 @@
     <t>1 example had a month of 'j' - this record was dropped. Majority in May</t>
   </si>
   <si>
-    <t>Poster</t>
-  </si>
-  <si>
-    <t>Make reference to following CRISP</t>
-  </si>
-  <si>
     <t>Unique-id. Flat &amp; wide so dropped. But 18 duplicated, flag for later resolution</t>
   </si>
   <si>
@@ -234,12 +204,6 @@
     <t>Outlier of 275 was dropped. 40k not contacted, majority under 10 (96%)</t>
   </si>
   <si>
-    <t>RobustScaler used due to outliers and skewed data</t>
-  </si>
-  <si>
-    <t>?? Which pre and post data item to show</t>
-  </si>
-  <si>
     <t>NB: Dropped after first modelling attempt</t>
   </si>
   <si>
@@ -256,15 +220,6 @@
   </si>
   <si>
     <t>Removed outliers &gt; 30. 76. But no impact on model so left</t>
-  </si>
-  <si>
-    <t>Appled outliers but mad little diffeence goven scaling and balancing in the models …. !! An insight</t>
-  </si>
-  <si>
-    <t>?? So not sure what data changed to show now!</t>
-  </si>
-  <si>
-    <t>?? SMOTE (Synhthetic Minority Over-Sampling Technique) - see 2002 paper</t>
   </si>
   <si>
     <t>Out of 20 original variables, 11 were retained. Including the single target binary classifiction.</t>
@@ -447,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -478,17 +433,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -832,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0774E0-D8AF-8F4A-A91C-6B13DF09BE6A}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -850,7 +798,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -864,10 +812,10 @@
         <v>22</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>23</v>
@@ -890,7 +838,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="14"/>
       <c r="G5" s="5" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -904,11 +852,11 @@
         <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -923,11 +871,11 @@
       </c>
       <c r="E7" s="2"/>
       <c r="G7" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="25"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
@@ -942,7 +890,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="25"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
@@ -955,11 +903,11 @@
       <c r="E9" s="2"/>
       <c r="F9" s="14"/>
       <c r="G9" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="25"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
@@ -974,7 +922,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="25"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
@@ -987,7 +935,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="14"/>
       <c r="G11" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1003,11 +951,11 @@
       <c r="E12" s="2"/>
       <c r="F12" s="14"/>
       <c r="G12" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="25"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="15" t="s">
         <v>8</v>
       </c>
@@ -1018,15 +966,15 @@
         <v>26</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="26"/>
+        <v>59</v>
+      </c>
+      <c r="F13" s="23"/>
       <c r="G13" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
@@ -1039,11 +987,11 @@
       <c r="E14" s="2"/>
       <c r="F14" s="14"/>
       <c r="G14" s="5" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="25"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="15" t="s">
         <v>10</v>
       </c>
@@ -1060,7 +1008,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="25"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="15" t="s">
         <v>11</v>
       </c>
@@ -1089,7 +1037,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="14"/>
       <c r="G17" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1097,7 +1045,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>27</v>
@@ -1121,11 +1069,11 @@
       <c r="E19" s="2"/>
       <c r="F19" s="14"/>
       <c r="G19" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="25"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="15" t="s">
         <v>15</v>
       </c>
@@ -1136,11 +1084,11 @@
         <v>26</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1170,11 +1118,11 @@
       </c>
       <c r="E22" s="2"/>
       <c r="G22" s="5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="25"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="6" t="s">
         <v>18</v>
       </c>
@@ -1185,10 +1133,10 @@
         <v>26</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1204,7 +1152,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="13"/>
       <c r="G24" s="9" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1214,10 +1162,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1235,7 +1183,7 @@
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="27">
+      <c r="C30" s="24">
         <v>50660</v>
       </c>
       <c r="D30" s="17">
@@ -1243,119 +1191,17 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C31" s="24">
+      <c r="C31" s="21">
         <f>C29-C30</f>
         <v>2</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31" s="21">
         <f>D29-D30</f>
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="22"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="21"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D40" s="21"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="18"/>
-      <c r="D41" s="21"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="18"/>
-      <c r="D43" s="21"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" s="21"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="21"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B46" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D48" s="21"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="18"/>
-      <c r="D49" s="21"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D50" s="20"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B51" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D51" s="20"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B52" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D52" s="20"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D53" s="20"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B54" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D54" s="20"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D55" s="20"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D56" s="20"/>
-    </row>
-    <row r="57" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B57" s="23"/>
+    <row r="34" spans="2:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="B34" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1383,7 +1229,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1397,10 +1243,10 @@
         <v>22</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>23</v>
@@ -1423,7 +1269,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="14"/>
       <c r="G5" s="5" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1437,11 +1283,11 @@
         <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1456,11 +1302,11 @@
       </c>
       <c r="E7" s="2"/>
       <c r="G7" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="25"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1475,7 +1321,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="25"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1488,11 +1334,11 @@
       <c r="E9" s="2"/>
       <c r="F9" s="14"/>
       <c r="G9" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="25"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1507,7 +1353,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="25"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
@@ -1520,7 +1366,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="14"/>
       <c r="G11" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1536,11 +1382,11 @@
       <c r="E12" s="2"/>
       <c r="F12" s="14"/>
       <c r="G12" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="25"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="15" t="s">
         <v>8</v>
       </c>
@@ -1551,15 +1397,15 @@
         <v>26</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="26"/>
+        <v>59</v>
+      </c>
+      <c r="F13" s="23"/>
       <c r="G13" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
@@ -1572,11 +1418,11 @@
       <c r="E14" s="2"/>
       <c r="F14" s="14"/>
       <c r="G14" s="5" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="25"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="15" t="s">
         <v>10</v>
       </c>
@@ -1593,7 +1439,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="25"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="15" t="s">
         <v>11</v>
       </c>
@@ -1622,7 +1468,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="14"/>
       <c r="G17" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1630,7 +1476,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>27</v>
@@ -1654,11 +1500,11 @@
       <c r="E19" s="2"/>
       <c r="F19" s="14"/>
       <c r="G19" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="25"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="15" t="s">
         <v>15</v>
       </c>
@@ -1669,11 +1515,11 @@
         <v>26</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1703,11 +1549,11 @@
       </c>
       <c r="E22" s="2"/>
       <c r="G22" s="5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="25"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="6" t="s">
         <v>18</v>
       </c>
@@ -1718,10 +1564,10 @@
         <v>26</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1737,20 +1583,20 @@
       <c r="E24" s="8"/>
       <c r="F24" s="13"/>
       <c r="G24" s="9" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D26" s="20"/>
+      <c r="D26" s="19"/>
     </row>
     <row r="27" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="B27" s="23" t="s">
-        <v>76</v>
+      <c r="B27" s="20" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>